<commit_message>
Added NFC reader BOM sheet
</commit_message>
<xml_diff>
--- a/BOMs/Consolidated_BOM.xlsx
+++ b/BOMs/Consolidated_BOM.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajeeth\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="159" documentId="8_{C8D15509-D721-4CB9-B7F7-2A36CF876BDA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{EE4CBBA9-FBBA-46E2-9979-A6779C561562}"/>
+  <xr:revisionPtr revIDLastSave="201" documentId="8_{C8D15509-D721-4CB9-B7F7-2A36CF876BDA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{81401B49-E525-4D18-8D82-4C31BFD3803E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3F0C4204-9B2B-4016-97A0-4C2BAD4064BB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{3F0C4204-9B2B-4016-97A0-4C2BAD4064BB}"/>
   </bookViews>
   <sheets>
     <sheet name="MainBoard_BOM" sheetId="1" r:id="rId1"/>
     <sheet name="LIDBoard_BOM" sheetId="2" r:id="rId2"/>
     <sheet name="LED_SENSE_BOM" sheetId="3" r:id="rId3"/>
     <sheet name="LED_Strip_BOM" sheetId="4" r:id="rId4"/>
+    <sheet name="NFC_READER" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="384">
   <si>
     <t>Manufacturer Part Number</t>
   </si>
@@ -60,15 +61,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>20021111-00010T4LF</t>
-  </si>
-  <si>
-    <t>Amphenol ICC (FCI)</t>
-  </si>
-  <si>
-    <t>609-3712-ND</t>
-  </si>
-  <si>
     <t>J4, J6</t>
   </si>
   <si>
@@ -81,9 +73,6 @@
     <t>Texas Instruments</t>
   </si>
   <si>
-    <t>296-47158-2-ND</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -165,33 +154,15 @@
     <t>CAP CER 4.7UF 6.3V X5R 0402</t>
   </si>
   <si>
-    <t>GRM21BR61C226ME44L</t>
-  </si>
-  <si>
-    <t>490-10747-1-ND</t>
-  </si>
-  <si>
     <t>C11</t>
   </si>
   <si>
     <t>CAP CER 22UF 16V X5R 0805</t>
   </si>
   <si>
-    <t>CDBUR0140L</t>
-  </si>
-  <si>
-    <t>Comchip Technology</t>
-  </si>
-  <si>
-    <t>641-1137-1-ND</t>
-  </si>
-  <si>
     <t>D1, D4</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 40V 100MA 0603</t>
-  </si>
-  <si>
     <t>CRCW04021K00JNED</t>
   </si>
   <si>
@@ -219,27 +190,15 @@
     <t>RES SMD 2.2K OHM 5% 1/16W 0402</t>
   </si>
   <si>
-    <t>RC0402JR-0710KL</t>
-  </si>
-  <si>
     <t>Yageo</t>
   </si>
   <si>
-    <t>311-10KJRCT-ND</t>
-  </si>
-  <si>
     <t>R38, R55, R56</t>
   </si>
   <si>
     <t>RES SMD 10K OHM 5% 1/16W 0402</t>
   </si>
   <si>
-    <t>RC0402JR-07100KL</t>
-  </si>
-  <si>
-    <t>311-100KJRCT-ND</t>
-  </si>
-  <si>
     <t>R13, R34, R35, R36, R53, R72</t>
   </si>
   <si>
@@ -267,9 +226,6 @@
     <t>P0.0JCT-ND</t>
   </si>
   <si>
-    <t>'R1, R2, R3, R4, R5, R6, R7, R8, R9, R10, R11, R12, R14, R15, R16, R17, R18, R19, R20, R21, R23, R25, R26, R27, R28, R29, R31, R51, R54, R58, R64, R66, R67, R68, R69, R70</t>
-  </si>
-  <si>
     <t>RES SMD 0 OHM JUMPER 1/10W 0402</t>
   </si>
   <si>
@@ -279,9 +235,6 @@
     <t>490-4539-1-ND</t>
   </si>
   <si>
-    <t>C5, C14, C15</t>
-  </si>
-  <si>
     <t>CAP CER 100UF 6.3V X5R 1206</t>
   </si>
   <si>
@@ -300,9 +253,6 @@
     <t>GRM3195C1H273JA01D</t>
   </si>
   <si>
-    <t>490-1762-1-ND</t>
-  </si>
-  <si>
     <t>C4, C17, C18, C19</t>
   </si>
   <si>
@@ -312,9 +262,6 @@
     <t>MLF2012C101KTD25</t>
   </si>
   <si>
-    <t>445-173938-1-ND</t>
-  </si>
-  <si>
     <t>L4, L5</t>
   </si>
   <si>
@@ -324,9 +271,6 @@
     <t>NC7WZ17P6X</t>
   </si>
   <si>
-    <t>NC7WZ17P6XCT-ND</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
@@ -336,9 +280,6 @@
     <t>RC0402FR-074K7L</t>
   </si>
   <si>
-    <t>311-4.7KLRCT-ND</t>
-  </si>
-  <si>
     <t>R48, R49</t>
   </si>
   <si>
@@ -348,9 +289,6 @@
     <t>RC0603JR-070RL</t>
   </si>
   <si>
-    <t>311-0.0GRCT-ND</t>
-  </si>
-  <si>
     <t>R30, R33, R39, R40, R41</t>
   </si>
   <si>
@@ -387,9 +325,6 @@
     <t>Sensirion AG</t>
   </si>
   <si>
-    <t>1649-1009-1-ND</t>
-  </si>
-  <si>
     <t>U5</t>
   </si>
   <si>
@@ -411,12 +346,6 @@
     <t>LED RED CLEAR 0603 SMD</t>
   </si>
   <si>
-    <t>TPS62162DSGR</t>
-  </si>
-  <si>
-    <t>296-43671-1-ND</t>
-  </si>
-  <si>
     <t>U3</t>
   </si>
   <si>
@@ -429,9 +358,6 @@
     <t>Semtech Corporation</t>
   </si>
   <si>
-    <t>UCLAMP0501HCT-ND</t>
-  </si>
-  <si>
     <t>D5</t>
   </si>
   <si>
@@ -450,30 +376,12 @@
     <t>TVS DIODE 3.3V 8V SOD523</t>
   </si>
   <si>
-    <t>0402ZD104KAT4A</t>
-  </si>
-  <si>
-    <t>AVX Corporation</t>
-  </si>
-  <si>
-    <t>478-11506-1-ND</t>
-  </si>
-  <si>
     <t>C9, C10, C20</t>
   </si>
   <si>
-    <t>GRM21BR61C106KE15K</t>
-  </si>
-  <si>
-    <t>490-6473-1-ND</t>
-  </si>
-  <si>
     <t>C12, C13</t>
   </si>
   <si>
-    <t>CAP CER 10UF 16V X5R 0805</t>
-  </si>
-  <si>
     <t>EAST1616RGBA8</t>
   </si>
   <si>
@@ -483,12 +391,6 @@
     <t>D3</t>
   </si>
   <si>
-    <t>LED, Rgb, SMD</t>
-  </si>
-  <si>
-    <t>'SimpleLink Wi-Fi and Internet-of-Things Module Solution, a Single-Chip Wireless MCU, MON0063A (QFM-63)</t>
-  </si>
-  <si>
     <t>AT42QT1010-TSHR</t>
   </si>
   <si>
@@ -621,15 +523,6 @@
     <t>SENSOR OPTICAL 200CM I2C</t>
   </si>
   <si>
-    <t>17.08(upto 100)</t>
-  </si>
-  <si>
-    <t>Price(upto 100 units)</t>
-  </si>
-  <si>
-    <t>Price(upto 10K)</t>
-  </si>
-  <si>
     <t>Designator</t>
   </si>
   <si>
@@ -1009,13 +902,301 @@
   </si>
   <si>
     <t>Manufacturer PartNumber</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>GRM188R71H102KA01D</t>
+  </si>
+  <si>
+    <t>490-1494-6-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 1000PF 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>C10, C11, C12, C13, C14, C15</t>
+  </si>
+  <si>
+    <t>C1608X5R1H105K080AB</t>
+  </si>
+  <si>
+    <t>445-7468-6-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 50V X5R 0603</t>
+  </si>
+  <si>
+    <t>C2, C3, C4, C7, C8</t>
+  </si>
+  <si>
+    <t>C1, C5</t>
+  </si>
+  <si>
+    <t>C0402C120J5GACTU</t>
+  </si>
+  <si>
+    <t>399-1013-6-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 12PF 50V C0G/NP0 0402</t>
+  </si>
+  <si>
+    <t>$9.80</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>EMK105BJ105KV-F</t>
+  </si>
+  <si>
+    <t>587-2477-6-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 16V X5R 0402</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>Bourns Inc.</t>
+  </si>
+  <si>
+    <t>CM453232-102KL</t>
+  </si>
+  <si>
+    <t>CM453232-102KLCT-ND</t>
+  </si>
+  <si>
+    <t>FIXED IND 1MH 30MA 40 OHM SMD</t>
+  </si>
+  <si>
+    <t>R1, R10, R11, R14, R15</t>
+  </si>
+  <si>
+    <t>R2, R3, R4, R8, R9, R13</t>
+  </si>
+  <si>
+    <t>541-10KJDKR-ND</t>
+  </si>
+  <si>
+    <t>$10.40</t>
+  </si>
+  <si>
+    <t>R5, R7, R12</t>
+  </si>
+  <si>
+    <t>BLM15AG102SN1D</t>
+  </si>
+  <si>
+    <t>490-1007-2-ND</t>
+  </si>
+  <si>
+    <t>FERRITE BEAD 1 KOHM 0402 1LN</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF2701X</t>
+  </si>
+  <si>
+    <t>P2.70KLTR-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 2.7K OHM 1% 1/10W 0402</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>ECS Inc.</t>
+  </si>
+  <si>
+    <t>ECS-271.2-10-37-CKM-TR</t>
+  </si>
+  <si>
+    <t>XC2511DKR-ND</t>
+  </si>
+  <si>
+    <t>CRYSTAL 27.12MHZ 10PF SMD</t>
+  </si>
+  <si>
+    <t>NXP USA Inc.</t>
+  </si>
+  <si>
+    <t>MFRC52202HN1,151</t>
+  </si>
+  <si>
+    <t>568-8603-ND</t>
+  </si>
+  <si>
+    <t>IC RFID READER 13.56MHZ 32HVQFN</t>
+  </si>
+  <si>
+    <t>$0.60</t>
+  </si>
+  <si>
+    <t>C2012X5R1C226K125AC</t>
+  </si>
+  <si>
+    <t>445-6797-1-ND</t>
+  </si>
+  <si>
+    <t>GRM21BR61A106KE19L</t>
+  </si>
+  <si>
+    <t>490-1709-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 10V X5R 0805</t>
+  </si>
+  <si>
+    <t>490-1762-6-ND</t>
+  </si>
+  <si>
+    <t>$12.58</t>
+  </si>
+  <si>
+    <t>$2.19</t>
+  </si>
+  <si>
+    <t>C1005X5R1A104K050BA</t>
+  </si>
+  <si>
+    <t>445-1265-1-ND</t>
+  </si>
+  <si>
+    <t>CD0603-B0240R</t>
+  </si>
+  <si>
+    <t>CD0603-B0240RTR-ND</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 40V 200MA 0603</t>
+  </si>
+  <si>
+    <t>$0.64</t>
+  </si>
+  <si>
+    <t>UCLAMP0501HDKR-ND</t>
+  </si>
+  <si>
+    <t>FID1, FID3, FID4</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>$2.50</t>
+  </si>
+  <si>
+    <t>Samtec Inc.</t>
+  </si>
+  <si>
+    <t>FTSH-105-01-F-D-K</t>
+  </si>
+  <si>
+    <t>SAM8909-ND</t>
+  </si>
+  <si>
+    <t>$8.08</t>
+  </si>
+  <si>
+    <t>$0.30</t>
+  </si>
+  <si>
+    <t>$0.51</t>
+  </si>
+  <si>
+    <t>445-173938-6-ND</t>
+  </si>
+  <si>
+    <t>$10.34</t>
+  </si>
+  <si>
+    <t>$1.44</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4, R5, R6, R7, R8, R9, R10, R11, R12, R14, R15, R16, R17, R18, R19, R20, R21, R23, R25, R26, R27, R28, R29, R31, R51, R54, R58, R64, R66, R67, R68, R69, R70</t>
+  </si>
+  <si>
+    <t>$1.19</t>
+  </si>
+  <si>
+    <t>CRCW0402100KJNED</t>
+  </si>
+  <si>
+    <t>541-100KJCT-ND</t>
+  </si>
+  <si>
+    <t>$0.90</t>
+  </si>
+  <si>
+    <t>R22, R24</t>
+  </si>
+  <si>
+    <t>311-0.0GRDKR-ND</t>
+  </si>
+  <si>
+    <t>$10.25</t>
+  </si>
+  <si>
+    <t>$0.45</t>
+  </si>
+  <si>
+    <t>311-4.7KLRDKR-ND</t>
+  </si>
+  <si>
+    <t>296-47158-1-ND</t>
+  </si>
+  <si>
+    <t>$32.55</t>
+  </si>
+  <si>
+    <t>NC7WZ17P6XTR-ND</t>
+  </si>
+  <si>
+    <t>TPS62162DSGT</t>
+  </si>
+  <si>
+    <t>296-29897-1-ND</t>
+  </si>
+  <si>
+    <t>$3.18</t>
+  </si>
+  <si>
+    <t>1649-1009-6-ND</t>
+  </si>
+  <si>
+    <t>$15.57</t>
+  </si>
+  <si>
+    <t>$4.26</t>
+  </si>
+  <si>
+    <t>CD0603-B00340</t>
+  </si>
+  <si>
+    <t>CD0603-B00340CT-ND</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 40V 30MA 0603</t>
+  </si>
+  <si>
+    <t>$1.02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1035,12 +1216,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1065,6 +1240,17 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1117,41 +1303,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{0A3F1A26-05A0-4D02-B2A2-89C842BE20BD}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1465,17 +1656,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB659AB9-5E9E-4EE4-8944-84B8330C54F7}">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" customWidth="1"/>
-    <col min="5" max="5" width="64" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" customWidth="1"/>
+    <col min="5" max="5" width="56.28515625" customWidth="1"/>
     <col min="6" max="6" width="16.140625" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
@@ -1484,36 +1675,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>197</v>
-      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="3"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -1522,29 +1709,29 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2">
-        <v>2</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0.97</v>
-      </c>
-      <c r="H2" s="2">
-        <v>1.94</v>
+      <c r="A2" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="15">
+        <v>4</v>
+      </c>
+      <c r="G2" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>333</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -1556,29 +1743,29 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
+      <c r="A3" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>334</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>335</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="15">
+        <v>1</v>
+      </c>
+      <c r="G3" s="15">
+        <v>0.30654999999999999</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>178</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1590,29 +1777,29 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="A4" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="H4" s="2">
-        <v>2.5</v>
+      <c r="C4" s="15" t="s">
+        <v>336</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>338</v>
+      </c>
+      <c r="F4" s="15">
+        <v>2</v>
+      </c>
+      <c r="G4" s="16">
+        <v>7.9750000000000001E-2</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>178</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -1624,29 +1811,29 @@
       <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="2">
-        <v>2</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0.3</v>
+      <c r="A5" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="15">
+        <v>4</v>
+      </c>
+      <c r="G5" s="15">
+        <v>3.145</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>340</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1658,29 +1845,29 @@
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0.51</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0.51</v>
+      <c r="A6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="15">
+        <v>3</v>
+      </c>
+      <c r="G6" s="15">
+        <v>0.73</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>341</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1692,29 +1879,29 @@
       <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="A7" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="C7" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="15">
         <v>3</v>
       </c>
-      <c r="G7" s="2">
-        <v>0.48</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1.44</v>
+      <c r="G7" s="15">
+        <v>0</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>178</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1726,29 +1913,29 @@
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="2">
-        <v>3</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0.73</v>
-      </c>
-      <c r="H8" s="2">
-        <v>2.19</v>
+      <c r="B8" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>121</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1760,29 +1947,29 @@
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0.7</v>
+      <c r="A9" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="15">
+        <v>1</v>
+      </c>
+      <c r="G9" s="15">
+        <v>0.64</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>347</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1794,29 +1981,29 @@
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="2">
-        <v>2</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="H10" s="2">
-        <v>1.4</v>
+      <c r="A10" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" s="15">
+        <v>1</v>
+      </c>
+      <c r="G10" s="15">
+        <v>0.45</v>
+      </c>
+      <c r="H10" s="15">
+        <v>0.45</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1828,29 +2015,29 @@
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="2">
-        <v>1</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0.15</v>
+      <c r="A11" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>348</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11" s="15">
+        <v>1</v>
+      </c>
+      <c r="G11" s="15">
+        <v>10.4</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>315</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1862,29 +2049,29 @@
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0.15</v>
+      <c r="A12" s="15" t="s">
+        <v>349</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>350</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>121</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1896,29 +2083,29 @@
       <c r="P12" s="2"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" s="2">
-        <v>3</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0.45</v>
+      <c r="A13" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="15">
+        <v>1</v>
+      </c>
+      <c r="G13" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>351</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1930,29 +2117,29 @@
       <c r="P13" s="2"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F14" s="2">
-        <v>6</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H14" s="2">
-        <v>0.9</v>
+      <c r="A14" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="15">
+        <v>2</v>
+      </c>
+      <c r="G14" s="15">
+        <v>4.04</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>355</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1964,29 +2151,29 @@
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" s="2">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2">
+      <c r="A15" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="15">
+        <v>2</v>
+      </c>
+      <c r="G15" s="15">
         <v>0.15</v>
       </c>
-      <c r="H15" s="2">
-        <v>0.15</v>
+      <c r="H15" s="15" t="s">
+        <v>356</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1998,29 +2185,29 @@
       <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F16" s="2">
-        <v>36</v>
-      </c>
-      <c r="G16" s="2">
-        <v>3.32E-2</v>
-      </c>
-      <c r="H16" s="2">
-        <v>1.19</v>
+      <c r="A16" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="15">
+        <v>1</v>
+      </c>
+      <c r="G16" s="15">
+        <v>0.51</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>357</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -2032,29 +2219,29 @@
       <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F17" s="2">
-        <v>3</v>
-      </c>
-      <c r="G17" s="2">
-        <v>1.42</v>
-      </c>
-      <c r="H17" s="2">
-        <v>4.26</v>
+      <c r="A17" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>358</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="15">
+        <v>2</v>
+      </c>
+      <c r="G17" s="15">
+        <v>5.17</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>359</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -2066,29 +2253,29 @@
       <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F18" s="2">
-        <v>4</v>
-      </c>
-      <c r="G18" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0.6</v>
+      <c r="A18" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="15">
+        <v>3</v>
+      </c>
+      <c r="G18" s="15">
+        <v>0.48</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>360</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -2100,29 +2287,29 @@
       <c r="P18" s="2"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F19" s="2">
-        <v>4</v>
-      </c>
-      <c r="G19" s="2">
-        <v>0.77</v>
-      </c>
-      <c r="H19" s="2">
-        <v>3.08</v>
+      <c r="A19" s="15" t="s">
+        <v>361</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="15">
+        <v>36</v>
+      </c>
+      <c r="G19" s="15">
+        <v>3.32E-2</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>362</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -2134,29 +2321,29 @@
       <c r="P19" s="2"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F20" s="2">
-        <v>2</v>
-      </c>
-      <c r="G20" s="2">
-        <v>0.42</v>
-      </c>
-      <c r="H20" s="2">
-        <v>0.84</v>
+      <c r="A20" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>364</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" s="15">
+        <v>6</v>
+      </c>
+      <c r="G20" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>365</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -2168,29 +2355,29 @@
       <c r="P20" s="2"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1</v>
-      </c>
-      <c r="G21" s="2">
-        <v>0.74</v>
-      </c>
-      <c r="H21" s="2">
-        <v>0.74</v>
+      <c r="A21" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" s="15">
+        <v>2</v>
+      </c>
+      <c r="G21" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>356</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -2202,29 +2389,29 @@
       <c r="P21" s="2"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F22" s="2">
-        <v>2</v>
-      </c>
-      <c r="G22" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H22" s="2">
-        <v>0.3</v>
+      <c r="A22" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>367</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="15">
+        <v>5</v>
+      </c>
+      <c r="G22" s="15">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>368</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -2236,29 +2423,29 @@
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F23" s="2">
-        <v>5</v>
-      </c>
-      <c r="G23" s="2">
+      <c r="A23" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="15">
+        <v>1</v>
+      </c>
+      <c r="G23" s="15">
         <v>0.15</v>
       </c>
-      <c r="H23" s="2">
-        <v>0.75</v>
+      <c r="H23" s="15" t="s">
+        <v>251</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -2270,29 +2457,29 @@
       <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F24" s="2">
-        <v>4</v>
-      </c>
-      <c r="G24" s="2">
+      <c r="A24" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="15">
+        <v>1</v>
+      </c>
+      <c r="G24" s="15">
         <v>0.15</v>
       </c>
-      <c r="H24" s="2">
-        <v>0.6</v>
+      <c r="H24" s="15" t="s">
+        <v>251</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -2304,29 +2491,29 @@
       <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F25" s="2">
-        <v>2</v>
-      </c>
-      <c r="G25" s="2">
+      <c r="A25" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="15">
+        <v>3</v>
+      </c>
+      <c r="G25" s="15">
         <v>0.15</v>
       </c>
-      <c r="H25" s="2">
-        <v>0.3</v>
+      <c r="H25" s="15" t="s">
+        <v>369</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -2338,29 +2525,29 @@
       <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F26" s="2">
-        <v>1</v>
-      </c>
-      <c r="G26" s="2">
-        <v>6.07</v>
-      </c>
-      <c r="H26" s="2">
-        <v>6.07</v>
+      <c r="A26" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" s="15">
+        <v>1</v>
+      </c>
+      <c r="G26" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>251</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -2372,29 +2559,29 @@
       <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F27" s="2">
-        <v>1</v>
-      </c>
-      <c r="G27" s="2">
-        <v>0.64</v>
-      </c>
-      <c r="H27" s="2">
-        <v>0.64</v>
+      <c r="A27" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>370</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" s="15">
+        <v>2</v>
+      </c>
+      <c r="G27" s="15">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>302</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -2406,29 +2593,29 @@
       <c r="P27" s="2"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F28" s="2">
-        <v>1</v>
-      </c>
-      <c r="G28" s="2">
-        <v>2.77</v>
-      </c>
-      <c r="H28" s="2">
-        <v>2.77</v>
+      <c r="A28" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28" s="15">
+        <v>4</v>
+      </c>
+      <c r="G28" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>333</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -2440,29 +2627,29 @@
       <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F29" s="2">
-        <v>1</v>
-      </c>
-      <c r="G29" s="2">
-        <v>0.94</v>
-      </c>
-      <c r="H29" s="2">
-        <v>0.94</v>
+      <c r="A29" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="15">
+        <v>1</v>
+      </c>
+      <c r="G29" s="15">
+        <v>32.549999999999997</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>372</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -2474,29 +2661,29 @@
       <c r="P29" s="2"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="F30" s="2">
-        <v>1</v>
-      </c>
-      <c r="G30" s="2">
-        <v>1.07</v>
-      </c>
-      <c r="H30" s="2">
-        <v>1.07</v>
+      <c r="A30" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>373</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F30" s="15">
+        <v>1</v>
+      </c>
+      <c r="G30" s="15">
+        <v>0.74</v>
+      </c>
+      <c r="H30" s="15" t="s">
+        <v>178</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -2508,29 +2695,29 @@
       <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F31" s="2">
-        <v>3</v>
-      </c>
-      <c r="G31" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H31" s="2">
-        <v>0.45</v>
+      <c r="A31" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>374</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>375</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" s="15">
+        <v>1</v>
+      </c>
+      <c r="G31" s="15">
+        <v>3.18</v>
+      </c>
+      <c r="H31" s="15" t="s">
+        <v>376</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -2542,29 +2729,29 @@
       <c r="P31" s="2"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F32" s="2">
-        <v>2</v>
-      </c>
-      <c r="G32" s="2">
-        <v>0.46</v>
-      </c>
-      <c r="H32" s="2">
-        <v>0.92</v>
+      <c r="A32" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="F32" s="15">
+        <v>1</v>
+      </c>
+      <c r="G32" s="15">
+        <v>15.57</v>
+      </c>
+      <c r="H32" s="15" t="s">
+        <v>378</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
@@ -2576,28 +2763,30 @@
       <c r="P32" s="2"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F33" s="2">
-        <v>1</v>
-      </c>
-      <c r="G33" s="2">
-        <v>0.45</v>
-      </c>
-      <c r="H33" s="2"/>
+      <c r="A33" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" s="15">
+        <v>3</v>
+      </c>
+      <c r="G33" s="15">
+        <v>1.42</v>
+      </c>
+      <c r="H33" s="15" t="s">
+        <v>379</v>
+      </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
@@ -2608,26 +2797,30 @@
       <c r="P33" s="2"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F34" s="2">
-        <v>1</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="H34" s="2"/>
+      <c r="A34" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>382</v>
+      </c>
+      <c r="F34" s="15">
+        <v>2</v>
+      </c>
+      <c r="G34" s="15">
+        <v>0</v>
+      </c>
+      <c r="H34" s="15" t="s">
+        <v>178</v>
+      </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
@@ -2637,11 +2830,34 @@
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
     </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F35" s="15">
+        <v>1</v>
+      </c>
+      <c r="G35" s="15">
+        <v>1.02</v>
+      </c>
+      <c r="H35" s="15" t="s">
+        <v>383</v>
+      </c>
+    </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H36" s="6">
-        <f>SUM(H2:H34)</f>
-        <v>38.300000000000004</v>
-      </c>
+      <c r="H36" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2654,7 +2870,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2669,46 +2885,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>203</v>
+        <v>167</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>204</v>
+        <v>168</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>159</v>
+        <v>126</v>
       </c>
       <c r="F2" s="2">
         <v>3</v>
@@ -2717,24 +2933,24 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>215</v>
+        <v>179</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>160</v>
+        <v>127</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>161</v>
+        <v>128</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>162</v>
+        <v>129</v>
       </c>
       <c r="F3" s="2">
         <v>2</v>
@@ -2743,24 +2959,24 @@
         <v>5.29</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>216</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>217</v>
+        <v>181</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>218</v>
+        <v>182</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>219</v>
+        <v>183</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>220</v>
+        <v>184</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
@@ -2769,24 +2985,24 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>221</v>
+        <v>185</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>157</v>
+        <v>124</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>222</v>
+        <v>186</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>223</v>
+        <v>187</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>224</v>
+        <v>188</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
@@ -2795,24 +3011,24 @@
         <v>10.050000000000001</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>225</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>226</v>
+        <v>190</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>227</v>
+        <v>191</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>228</v>
+        <v>192</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>229</v>
+        <v>193</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
@@ -2821,24 +3037,24 @@
         <v>0.36</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>230</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>231</v>
+        <v>195</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>232</v>
+        <v>196</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>233</v>
+        <v>197</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>234</v>
+        <v>198</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
@@ -2847,24 +3063,24 @@
         <v>0</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>235</v>
+        <v>199</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>236</v>
+        <v>200</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>237</v>
+        <v>201</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>238</v>
+        <v>202</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
@@ -2873,24 +3089,24 @@
         <v>0</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>239</v>
+        <v>203</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>240</v>
+        <v>204</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>241</v>
+        <v>205</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>242</v>
+        <v>206</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
@@ -2899,24 +3115,24 @@
         <v>9.65</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>243</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>192</v>
+        <v>159</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>244</v>
+        <v>208</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>245</v>
+        <v>209</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>246</v>
+        <v>210</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
@@ -2925,24 +3141,24 @@
         <v>10.17</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>247</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>250</v>
+        <v>214</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>251</v>
+        <v>215</v>
       </c>
       <c r="F11" s="2">
         <v>2</v>
@@ -2951,24 +3167,24 @@
         <v>0</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>252</v>
+        <v>216</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>253</v>
+        <v>217</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>254</v>
+        <v>218</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>255</v>
+        <v>219</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
@@ -2977,24 +3193,24 @@
         <v>0</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>256</v>
+        <v>220</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>257</v>
+        <v>221</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>258</v>
+        <v>222</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>259</v>
+        <v>223</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>260</v>
+        <v>224</v>
       </c>
       <c r="F13" s="2">
         <v>1</v>
@@ -3003,24 +3219,24 @@
         <v>4.3</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>261</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>262</v>
+        <v>226</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="F14" s="2">
         <v>2</v>
@@ -3029,24 +3245,24 @@
         <v>0</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>264</v>
+        <v>228</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>265</v>
+        <v>229</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>266</v>
+        <v>230</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>267</v>
+        <v>231</v>
       </c>
       <c r="F15" s="2">
         <v>1</v>
@@ -3055,24 +3271,24 @@
         <v>9.65</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>243</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>268</v>
+        <v>232</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>269</v>
+        <v>233</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>270</v>
+        <v>234</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>271</v>
+        <v>235</v>
       </c>
       <c r="F16" s="2">
         <v>1</v>
@@ -3081,24 +3297,24 @@
         <v>0</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>272</v>
+        <v>236</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>273</v>
+        <v>237</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>274</v>
+        <v>238</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>275</v>
+        <v>239</v>
       </c>
       <c r="F17" s="2">
         <v>1</v>
@@ -3107,24 +3323,24 @@
         <v>0</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>276</v>
+        <v>240</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>277</v>
+        <v>241</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>278</v>
+        <v>242</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>279</v>
+        <v>243</v>
       </c>
       <c r="F18" s="2">
         <v>1</v>
@@ -3133,24 +3349,24 @@
         <v>9.65</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>243</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>280</v>
+        <v>244</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="F19" s="2">
         <v>1</v>
@@ -3159,24 +3375,24 @@
         <v>9.65</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>243</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>284</v>
+        <v>248</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="F20" s="2">
         <v>1</v>
@@ -3185,24 +3401,24 @@
         <v>0.15</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>292</v>
+        <v>256</v>
       </c>
       <c r="F21" s="2">
         <v>1</v>
@@ -3211,24 +3427,24 @@
         <v>0</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>293</v>
+        <v>257</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>294</v>
+        <v>258</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>295</v>
+        <v>259</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>296</v>
+        <v>260</v>
       </c>
       <c r="F22" s="2">
         <v>1</v>
@@ -3237,76 +3453,76 @@
         <v>0</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>297</v>
+        <v>261</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>298</v>
+        <v>262</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>299</v>
+        <v>263</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>300</v>
+        <v>264</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>301</v>
+        <v>265</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>302</v>
+        <v>266</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>303</v>
+        <v>267</v>
       </c>
       <c r="F25" s="2">
         <v>1</v>
@@ -3315,24 +3531,24 @@
         <v>0</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>304</v>
+        <v>268</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>192</v>
+        <v>159</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>305</v>
+        <v>269</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>306</v>
+        <v>270</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>307</v>
+        <v>271</v>
       </c>
       <c r="F26" s="2">
         <v>1</v>
@@ -3341,7 +3557,7 @@
         <v>0</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -3351,10 +3567,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E60A712-8B68-43BC-805F-0841F2AA1E26}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3375,28 +3591,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="1"/>
@@ -3405,19 +3621,19 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>308</v>
+        <v>272</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>151</v>
+        <v>118</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>153</v>
+        <v>120</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="F2" s="2">
         <v>2</v>
@@ -3433,19 +3649,19 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>309</v>
+        <v>273</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>157</v>
+        <v>124</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>156</v>
+        <v>123</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>159</v>
+        <v>126</v>
       </c>
       <c r="F3" s="2">
         <v>5</v>
@@ -3461,19 +3677,19 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>310</v>
+        <v>274</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>160</v>
+        <v>127</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>161</v>
+        <v>128</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>162</v>
+        <v>129</v>
       </c>
       <c r="F4" s="2">
         <v>2</v>
@@ -3489,19 +3705,19 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>311</v>
+        <v>275</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>163</v>
+        <v>130</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>164</v>
+        <v>131</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>165</v>
+        <v>132</v>
       </c>
       <c r="F5" s="2">
         <v>2</v>
@@ -3517,19 +3733,19 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>312</v>
+        <v>276</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>166</v>
+        <v>133</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
@@ -3545,19 +3761,19 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>313</v>
+        <v>277</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>170</v>
+        <v>137</v>
       </c>
       <c r="F7" s="2">
         <v>4</v>
@@ -3573,19 +3789,19 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>314</v>
+        <v>278</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>172</v>
+        <v>139</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>173</v>
+        <v>140</v>
       </c>
       <c r="F8" s="2">
         <v>2</v>
@@ -3601,47 +3817,47 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>315</v>
+        <v>279</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>316</v>
+        <v>280</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>317</v>
+        <v>281</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>175</v>
+        <v>142</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>174</v>
+        <v>141</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>177</v>
+        <v>144</v>
       </c>
       <c r="F10" s="2">
         <v>6</v>
@@ -3657,19 +3873,19 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>178</v>
+        <v>145</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>179</v>
+        <v>146</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>180</v>
+        <v>147</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
@@ -3685,19 +3901,19 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>318</v>
+        <v>282</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>181</v>
+        <v>148</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>183</v>
+        <v>150</v>
       </c>
       <c r="F12" s="2">
         <v>2</v>
@@ -3713,19 +3929,19 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>319</v>
+        <v>283</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>184</v>
+        <v>151</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>185</v>
+        <v>152</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>186</v>
+        <v>153</v>
       </c>
       <c r="F13" s="2">
         <v>3</v>
@@ -3741,19 +3957,19 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>320</v>
+        <v>284</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>187</v>
+        <v>154</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>188</v>
+        <v>155</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>189</v>
+        <v>156</v>
       </c>
       <c r="F14" s="2">
         <v>2</v>
@@ -3769,47 +3985,47 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>321</v>
+        <v>285</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>190</v>
+        <v>157</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>322</v>
+        <v>286</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="F16" s="2">
         <v>5</v>
@@ -3825,19 +4041,19 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>323</v>
+        <v>287</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>192</v>
+        <v>159</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>191</v>
+        <v>158</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>193</v>
+        <v>160</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>194</v>
+        <v>161</v>
       </c>
       <c r="F17" s="2">
         <v>1</v>
@@ -3848,8 +4064,14 @@
       <c r="H17" s="2">
         <v>8.14</v>
       </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <f>SUM(H2:H17)</f>
+        <v>33.489999999999995</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3860,8 +4082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88BEB5F5-AB6B-4343-ABA4-5DE94416A3CA}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3879,61 +4101,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="F1" s="12" t="s">
+      <c r="A1" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="I1" s="13" t="s">
+      <c r="H1" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="F2" s="8">
+      <c r="A2" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F2" s="7">
         <v>21</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>206</v>
+      <c r="G2" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="I2">
         <v>1.975E-2</v>
@@ -3943,29 +4165,29 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="F3" s="8">
+      <c r="A3" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="F3" s="7">
         <v>22</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>212</v>
+      <c r="G3" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>176</v>
       </c>
       <c r="I3">
         <v>0.19</v>
@@ -3981,4 +4203,406 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15ECF306-7967-4B0E-BC66-B7827D078673}">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F3" s="2">
+        <v>6</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.94333</v>
+      </c>
+      <c r="H3" s="2">
+        <v>11.66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="H5" s="2">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2">
+        <v>9.65</v>
+      </c>
+      <c r="H6" s="2">
+        <v>9.65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="H9" s="13">
+        <v>9.6300000000000008</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="2">
+        <v>5</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="2">
+        <v>6</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1.73333</v>
+      </c>
+      <c r="H11" s="2">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="F12" s="2">
+        <v>3</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2">
+        <v>10.57</v>
+      </c>
+      <c r="H14" s="2">
+        <v>10.57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2">
+        <f>SUM(H2:H14)</f>
+        <v>62.85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Compiled and updated Consolidated BOM
</commit_message>
<xml_diff>
--- a/BOMs/Consolidated_BOM.xlsx
+++ b/BOMs/Consolidated_BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajeeth\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kashi\OneDrive - Airzai\Airzai\GitHub\Airzai-Hardware\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="208" documentId="8_{C8D15509-D721-4CB9-B7F7-2A36CF876BDA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{DF3DC6AD-C609-4669-8876-D89AFC8E2A8B}"/>
+  <xr:revisionPtr revIDLastSave="225" documentId="8_{C8D15509-D721-4CB9-B7F7-2A36CF876BDA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{DFD2C1A9-44D1-4B23-A56B-DD52AE2EDE42}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{3F0C4204-9B2B-4016-97A0-4C2BAD4064BB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="30915" windowHeight="15796" xr2:uid="{3F0C4204-9B2B-4016-97A0-4C2BAD4064BB}"/>
   </bookViews>
   <sheets>
     <sheet name="MainBoard_BOM" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="LED_Strip_BOM" sheetId="4" r:id="rId4"/>
     <sheet name="NFC_READER" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MainBoard_BOM!$A$1:$P$35</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="370">
   <si>
     <t>Manufacturer Part Number</t>
   </si>
@@ -997,12 +1000,6 @@
     <t>UCLAMP0501HDKR-ND</t>
   </si>
   <si>
-    <t>FID1, FID3, FID4</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Samtec Inc.</t>
   </si>
   <si>
@@ -1142,6 +1139,15 @@
   </si>
   <si>
     <t>$2.43</t>
+  </si>
+  <si>
+    <t>C5, C14, C15</t>
+  </si>
+  <si>
+    <t>RGB LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1155,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -1293,7 +1299,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1611,25 +1617,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB659AB9-5E9E-4EE4-8944-84B8330C54F7}">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" customWidth="1"/>
-    <col min="5" max="5" width="56.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="27.3984375" customWidth="1"/>
+    <col min="2" max="2" width="39.265625" customWidth="1"/>
+    <col min="3" max="3" width="30.3984375" customWidth="1"/>
+    <col min="4" max="4" width="34.3984375" customWidth="1"/>
+    <col min="5" max="5" width="56.265625" customWidth="1"/>
+    <col min="6" max="6" width="16.1328125" customWidth="1"/>
+    <col min="7" max="7" width="17.86328125" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="19.265625" customWidth="1"/>
+    <col min="10" max="10" width="18.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
@@ -1663,7 +1669,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" s="15" t="s">
         <v>69</v>
       </c>
@@ -1686,6 +1692,7 @@
         <v>0.15</v>
       </c>
       <c r="H2" s="15">
+        <f xml:space="preserve"> (F2*G2)</f>
         <v>0.6</v>
       </c>
       <c r="I2" s="2"/>
@@ -1697,7 +1704,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" s="15" t="s">
         <v>39</v>
       </c>
@@ -1720,7 +1727,8 @@
         <v>0.30654999999999999</v>
       </c>
       <c r="H3" s="15">
-        <v>0</v>
+        <f xml:space="preserve"> (F3*G3)</f>
+        <v>0.30654999999999999</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1731,7 +1739,7 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" s="15" t="s">
         <v>114</v>
       </c>
@@ -1754,7 +1762,8 @@
         <v>7.9750000000000001E-2</v>
       </c>
       <c r="H4" s="15">
-        <v>0</v>
+        <f xml:space="preserve"> (F4*G4)</f>
+        <v>0.1595</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -1765,7 +1774,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
         <v>72</v>
       </c>
@@ -1788,6 +1797,7 @@
         <v>3.145</v>
       </c>
       <c r="H5" s="15">
+        <f xml:space="preserve"> (F5*G5)</f>
         <v>12.58</v>
       </c>
       <c r="I5" s="2"/>
@@ -1799,30 +1809,31 @@
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>37</v>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>367</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="F6" s="15">
         <v>3</v>
       </c>
       <c r="G6" s="15">
-        <v>0.73</v>
+        <v>1.42</v>
       </c>
       <c r="H6" s="15">
-        <v>2.19</v>
+        <f xml:space="preserve"> (F6*G6)</f>
+        <v>4.26</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1833,30 +1844,31 @@
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7" s="15" t="s">
-        <v>113</v>
+        <v>37</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>314</v>
+        <v>34</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>315</v>
+        <v>36</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="F7" s="15">
         <v>3</v>
       </c>
       <c r="G7" s="15">
-        <v>0</v>
+        <v>0.73</v>
       </c>
       <c r="H7" s="15">
-        <v>0</v>
+        <f xml:space="preserve"> (F7*G7)</f>
+        <v>2.19</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1867,30 +1879,31 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" s="15" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>284</v>
+        <v>35</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>318</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>121</v>
+        <v>70</v>
+      </c>
+      <c r="F8" s="15">
+        <v>3</v>
+      </c>
+      <c r="G8" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="H8" s="15">
+        <f xml:space="preserve"> (F8*G8)</f>
+        <v>0.44999999999999996</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1901,30 +1914,31 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9" s="15" t="s">
-        <v>101</v>
+        <v>41</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>99</v>
+        <v>284</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>98</v>
+        <v>316</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>100</v>
+        <v>317</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>102</v>
+        <v>318</v>
       </c>
       <c r="F9" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9" s="15">
-        <v>0.64</v>
+        <v>0.7</v>
       </c>
       <c r="H9" s="15">
-        <v>0.64</v>
+        <f xml:space="preserve"> (F9*G9)</f>
+        <v>1.4</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1935,30 +1949,31 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10" s="15" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>116</v>
+        <v>284</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>115</v>
+        <v>335</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>121</v>
+        <v>336</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>121</v>
+        <v>337</v>
       </c>
       <c r="F10" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" s="15">
-        <v>0.45</v>
+        <v>0</v>
       </c>
       <c r="H10" s="15">
-        <v>0.45</v>
+        <f xml:space="preserve"> (F10*G10)</f>
+        <v>0</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1969,30 +1984,31 @@
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11" s="15" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>319</v>
+        <v>100</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F11" s="15">
         <v>1</v>
       </c>
       <c r="G11" s="15">
-        <v>10.4</v>
+        <v>0.64</v>
       </c>
       <c r="H11" s="15">
-        <v>10.4</v>
+        <f xml:space="preserve"> (F11*G11)</f>
+        <v>0.64</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -2003,30 +2019,31 @@
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12" s="15" t="s">
-        <v>320</v>
+        <v>117</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>321</v>
+        <v>115</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>121</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>121</v>
+        <v>368</v>
+      </c>
+      <c r="F12" s="15">
+        <v>1</v>
+      </c>
+      <c r="G12" s="15">
+        <v>0.45</v>
+      </c>
+      <c r="H12" s="15">
+        <f xml:space="preserve"> (F12*G12)</f>
+        <v>0.45</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -2037,30 +2054,31 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A13" s="15" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>15</v>
+        <v>106</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>14</v>
+        <v>105</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>16</v>
+        <v>319</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>18</v>
+        <v>108</v>
       </c>
       <c r="F13" s="15">
         <v>1</v>
       </c>
       <c r="G13" s="15">
-        <v>2.5</v>
+        <v>10.4</v>
       </c>
       <c r="H13" s="15">
-        <v>2.5</v>
+        <f xml:space="preserve"> (F13*G13)</f>
+        <v>10.4</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -2071,64 +2089,58 @@
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A14" s="15" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>322</v>
+        <v>106</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>323</v>
+        <v>109</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>324</v>
+        <v>110</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>9</v>
+        <v>112</v>
       </c>
       <c r="F14" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G14" s="15">
-        <v>4.04</v>
+        <v>1.02</v>
       </c>
       <c r="H14" s="15">
-        <v>8.08</v>
-      </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+        <f xml:space="preserve"> (F14*G14)</f>
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A15" s="15" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F15" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15" s="15">
-        <v>0.15</v>
+        <v>2.5</v>
       </c>
       <c r="H15" s="15">
-        <v>0.3</v>
+        <f xml:space="preserve"> (F15*G15)</f>
+        <v>2.5</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -2139,30 +2151,31 @@
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A16" s="15" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>25</v>
+        <v>320</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>24</v>
+        <v>321</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>26</v>
+        <v>322</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F16" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G16" s="15">
-        <v>0.51</v>
+        <v>4.04</v>
       </c>
       <c r="H16" s="15">
-        <v>0.51</v>
+        <f xml:space="preserve"> (F16*G16)</f>
+        <v>8.08</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -2173,30 +2186,31 @@
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A17" s="15" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>74</v>
+        <v>19</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>325</v>
+        <v>21</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="F17" s="15">
         <v>2</v>
       </c>
       <c r="G17" s="15">
-        <v>5.17</v>
+        <v>0.15</v>
       </c>
       <c r="H17" s="15">
-        <v>10.34</v>
+        <f xml:space="preserve"> (F17*G17)</f>
+        <v>0.3</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -2207,30 +2221,31 @@
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A18" s="15" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F18" s="15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G18" s="15">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
       <c r="H18" s="15">
-        <v>1.44</v>
+        <f xml:space="preserve"> (F18*G18)</f>
+        <v>0.51</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -2241,30 +2256,31 @@
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A19" s="15" t="s">
-        <v>326</v>
+        <v>75</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>62</v>
+        <v>323</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="F19" s="15">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="G19" s="15">
-        <v>3.32E-2</v>
+        <v>5.17</v>
       </c>
       <c r="H19" s="15">
-        <v>1.19</v>
+        <f xml:space="preserve"> (F19*G19)</f>
+        <v>10.34</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -2275,30 +2291,31 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A20" s="15" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>327</v>
+        <v>29</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>328</v>
+        <v>31</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="F20" s="15">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G20" s="15">
-        <v>0.15</v>
+        <v>0.48</v>
       </c>
       <c r="H20" s="15">
-        <v>0.9</v>
+        <f xml:space="preserve"> (F20*G20)</f>
+        <v>1.44</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -2309,30 +2326,31 @@
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A21" s="15" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="F21" s="15">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="G21" s="15">
-        <v>0.15</v>
+        <v>3.32E-2</v>
       </c>
       <c r="H21" s="15">
-        <v>0.3</v>
+        <f xml:space="preserve"> (F21*G21)</f>
+        <v>1.1952</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -2343,30 +2361,31 @@
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A22" s="15" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>83</v>
+        <v>325</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="F22" s="15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G22" s="15">
-        <v>2.0499999999999998</v>
+        <v>0.15</v>
       </c>
       <c r="H22" s="15">
-        <v>10.25</v>
+        <f xml:space="preserve"> (F22*G22)</f>
+        <v>0.89999999999999991</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -2377,30 +2396,31 @@
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23" s="15" t="s">
-        <v>58</v>
+        <v>327</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="F23" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G23" s="15">
         <v>0.15</v>
       </c>
       <c r="H23" s="15">
-        <v>0.15</v>
+        <f xml:space="preserve"> (F23*G23)</f>
+        <v>0.3</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -2411,30 +2431,31 @@
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24" s="15" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>48</v>
+        <v>328</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="F24" s="15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G24" s="15">
-        <v>0.15</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="H24" s="15">
-        <v>0.15</v>
+        <f xml:space="preserve"> (F24*G24)</f>
+        <v>10.25</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -2445,30 +2466,31 @@
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A25" s="15" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>43</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>230</v>
+        <v>56</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>231</v>
+        <v>57</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F25" s="15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G25" s="15">
         <v>0.15</v>
       </c>
       <c r="H25" s="15">
-        <v>0.45</v>
+        <f xml:space="preserve"> (F25*G25)</f>
+        <v>0.15</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -2479,21 +2501,21 @@
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A26" s="15" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F26" s="15">
         <v>1</v>
@@ -2502,6 +2524,7 @@
         <v>0.15</v>
       </c>
       <c r="H26" s="15">
+        <f xml:space="preserve"> (F26*G26)</f>
         <v>0.15</v>
       </c>
       <c r="I26" s="2"/>
@@ -2513,30 +2536,31 @@
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A27" s="15" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>80</v>
+        <v>230</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>331</v>
+        <v>231</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="F27" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G27" s="15">
-        <v>4.9000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="H27" s="15">
-        <v>9.8000000000000007</v>
+        <f xml:space="preserve"> (F27*G27)</f>
+        <v>0.44999999999999996</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -2547,30 +2571,31 @@
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A28" s="15" t="s">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>87</v>
+        <v>44</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="F28" s="15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G28" s="15">
         <v>0.15</v>
       </c>
       <c r="H28" s="15">
-        <v>0.6</v>
+        <f xml:space="preserve"> (F28*G28)</f>
+        <v>0.15</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -2581,30 +2606,31 @@
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A29" s="15" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="F29" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G29" s="15">
-        <v>32.549999999999997</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="H29" s="15">
-        <v>32.549999999999997</v>
+        <f xml:space="preserve"> (F29*G29)</f>
+        <v>9.8000000000000007</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -2615,30 +2641,31 @@
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A30" s="15" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>333</v>
+        <v>87</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="F30" s="15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G30" s="15">
-        <v>0.74</v>
+        <v>0.15</v>
       </c>
       <c r="H30" s="15">
-        <v>0</v>
+        <f xml:space="preserve"> (F30*G30)</f>
+        <v>0.6</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -2649,30 +2676,31 @@
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A31" s="15" t="s">
-        <v>103</v>
+        <v>12</v>
       </c>
       <c r="B31" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>334</v>
+        <v>10</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>104</v>
+        <v>13</v>
       </c>
       <c r="F31" s="15">
         <v>1</v>
       </c>
       <c r="G31" s="15">
-        <v>3.18</v>
+        <v>18</v>
       </c>
       <c r="H31" s="15">
-        <v>3.18</v>
+        <f xml:space="preserve"> (F31*G31)</f>
+        <v>18</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -2683,30 +2711,31 @@
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A32" s="15" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>95</v>
+        <v>30</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="F32" s="15">
         <v>1</v>
       </c>
       <c r="G32" s="15">
-        <v>15.57</v>
+        <v>0.74</v>
       </c>
       <c r="H32" s="15">
-        <v>15.57</v>
+        <f xml:space="preserve"> (F32*G32)</f>
+        <v>0.74</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
@@ -2717,30 +2746,31 @@
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A33" s="15" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>64</v>
+        <v>332</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>65</v>
+        <v>333</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>66</v>
+        <v>104</v>
       </c>
       <c r="F33" s="15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G33" s="15">
-        <v>1.42</v>
+        <v>3.18</v>
       </c>
       <c r="H33" s="15">
-        <v>4.26</v>
+        <f xml:space="preserve"> (F33*G33)</f>
+        <v>3.18</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -2751,30 +2781,31 @@
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A34" s="15" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>284</v>
+        <v>95</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>337</v>
+        <v>94</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>339</v>
+        <v>97</v>
       </c>
       <c r="F34" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G34" s="15">
-        <v>0</v>
+        <v>15.57</v>
       </c>
       <c r="H34" s="15">
-        <v>0</v>
+        <f xml:space="preserve"> (F34*G34)</f>
+        <v>15.57</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
@@ -2785,39 +2816,24 @@
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="F35" s="15">
-        <v>1</v>
-      </c>
-      <c r="G35" s="15">
-        <v>1.02</v>
-      </c>
-      <c r="H35" s="15">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H36" s="5">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="G36" t="s">
+        <v>369</v>
+      </c>
+      <c r="H36" s="15">
         <f>SUM(H2:H35)</f>
-        <v>130.54999999999998</v>
+        <v>119.06125</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:P35" xr:uid="{7615D240-7B10-4729-8CBD-C77B1850A1C1}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P35">
+      <sortCondition ref="A1:A35"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -2831,18 +2847,18 @@
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.86328125" customWidth="1"/>
+    <col min="2" max="2" width="33.1328125" customWidth="1"/>
+    <col min="3" max="3" width="28.73046875" customWidth="1"/>
+    <col min="4" max="4" width="28.3984375" customWidth="1"/>
+    <col min="5" max="5" width="41.3984375" customWidth="1"/>
+    <col min="7" max="7" width="16.86328125" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -2868,7 +2884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>177</v>
       </c>
@@ -2891,10 +2907,10 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>178</v>
       </c>
@@ -2917,10 +2933,10 @@
         <v>5.29</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>179</v>
       </c>
@@ -2943,10 +2959,10 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>183</v>
       </c>
@@ -2957,7 +2973,7 @@
         <v>184</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>185</v>
@@ -2969,10 +2985,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>186</v>
       </c>
@@ -2995,10 +3011,10 @@
         <v>0.36</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>190</v>
       </c>
@@ -3009,7 +3025,7 @@
         <v>191</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>192</v>
@@ -3021,10 +3037,10 @@
         <v>1.28</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>193</v>
       </c>
@@ -3035,7 +3051,7 @@
         <v>194</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>195</v>
@@ -3047,10 +3063,10 @@
         <v>0.35</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>196</v>
       </c>
@@ -3061,7 +3077,7 @@
         <v>197</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>198</v>
@@ -3073,10 +3089,10 @@
         <v>0.15</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>117</v>
       </c>
@@ -3087,7 +3103,7 @@
         <v>199</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>200</v>
@@ -3099,10 +3115,10 @@
         <v>0.67</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>201</v>
       </c>
@@ -3113,7 +3129,7 @@
         <v>202</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>203</v>
@@ -3125,10 +3141,10 @@
         <v>0.89</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>204</v>
       </c>
@@ -3139,7 +3155,7 @@
         <v>205</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>206</v>
@@ -3151,10 +3167,10 @@
         <v>1.39</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>207</v>
       </c>
@@ -3177,10 +3193,10 @@
         <v>4.3</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>212</v>
       </c>
@@ -3203,10 +3219,10 @@
         <v>0.15</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>214</v>
       </c>
@@ -3217,7 +3233,7 @@
         <v>215</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>216</v>
@@ -3229,10 +3245,10 @@
         <v>0.15</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>217</v>
       </c>
@@ -3243,7 +3259,7 @@
         <v>218</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>219</v>
@@ -3255,10 +3271,10 @@
         <v>0.15</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>220</v>
       </c>
@@ -3269,7 +3285,7 @@
         <v>221</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>222</v>
@@ -3281,10 +3297,10 @@
         <v>0.15</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>223</v>
       </c>
@@ -3295,7 +3311,7 @@
         <v>224</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>225</v>
@@ -3307,10 +3323,10 @@
         <v>0.15</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>226</v>
       </c>
@@ -3321,7 +3337,7 @@
         <v>227</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>228</v>
@@ -3333,10 +3349,10 @@
         <v>0.15</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>229</v>
       </c>
@@ -3359,10 +3375,10 @@
         <v>0.15</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>232</v>
       </c>
@@ -3373,7 +3389,7 @@
         <v>234</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>235</v>
@@ -3385,10 +3401,10 @@
         <v>0.15</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>236</v>
       </c>
@@ -3399,7 +3415,7 @@
         <v>237</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>238</v>
@@ -3411,10 +3427,10 @@
         <v>0.33</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>239</v>
       </c>
@@ -3440,7 +3456,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>241</v>
       </c>
@@ -3466,7 +3482,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>96</v>
       </c>
@@ -3489,10 +3505,10 @@
         <v>0</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>246</v>
       </c>
@@ -3503,7 +3519,7 @@
         <v>247</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>248</v>
@@ -3515,7 +3531,7 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -3531,24 +3547,24 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="33.3984375" customWidth="1"/>
+    <col min="3" max="3" width="25.3984375" customWidth="1"/>
+    <col min="4" max="4" width="23.59765625" customWidth="1"/>
+    <col min="5" max="5" width="33.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.59765625" customWidth="1"/>
+    <col min="7" max="7" width="24.86328125" customWidth="1"/>
+    <col min="8" max="8" width="14.1328125" customWidth="1"/>
+    <col min="9" max="9" width="12.59765625" customWidth="1"/>
+    <col min="10" max="10" width="17.265625" customWidth="1"/>
+    <col min="11" max="11" width="17.59765625" customWidth="1"/>
+    <col min="12" max="12" width="15.265625" customWidth="1"/>
+    <col min="13" max="13" width="14.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -3577,7 +3593,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>249</v>
       </c>
@@ -3605,7 +3621,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>250</v>
       </c>
@@ -3633,7 +3649,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>251</v>
       </c>
@@ -3661,7 +3677,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>252</v>
       </c>
@@ -3689,7 +3705,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>253</v>
       </c>
@@ -3717,7 +3733,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>254</v>
       </c>
@@ -3745,7 +3761,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>255</v>
       </c>
@@ -3773,7 +3789,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>256</v>
       </c>
@@ -3801,7 +3817,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>258</v>
       </c>
@@ -3829,7 +3845,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>103</v>
       </c>
@@ -3857,7 +3873,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>259</v>
       </c>
@@ -3885,7 +3901,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>260</v>
       </c>
@@ -3913,7 +3929,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>261</v>
       </c>
@@ -3941,7 +3957,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>262</v>
       </c>
@@ -3969,7 +3985,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>263</v>
       </c>
@@ -3997,7 +4013,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>264</v>
       </c>
@@ -4025,7 +4041,7 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H18">
         <f>SUM(H2:H17)</f>
         <v>33.489999999999995</v>
@@ -4044,21 +4060,21 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="42.140625" customWidth="1"/>
+    <col min="1" max="1" width="42.1328125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.1328125" customWidth="1"/>
+    <col min="4" max="4" width="12.59765625" customWidth="1"/>
+    <col min="5" max="5" width="21.265625" customWidth="1"/>
+    <col min="6" max="6" width="10.1328125" customWidth="1"/>
+    <col min="7" max="7" width="16.59765625" customWidth="1"/>
+    <col min="8" max="8" width="14.1328125" customWidth="1"/>
+    <col min="9" max="9" width="13.86328125" customWidth="1"/>
+    <col min="10" max="10" width="15.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="10" t="s">
         <v>162</v>
       </c>
@@ -4090,7 +4106,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>166</v>
       </c>
@@ -4122,7 +4138,7 @@
         <v>0.41370000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
         <v>171</v>
       </c>
@@ -4167,22 +4183,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15ECF306-7967-4B0E-BC66-B7827D078673}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.59765625" customWidth="1"/>
+    <col min="3" max="3" width="26.3984375" customWidth="1"/>
+    <col min="4" max="4" width="22.3984375" customWidth="1"/>
+    <col min="5" max="5" width="35.3984375" customWidth="1"/>
+    <col min="7" max="7" width="15.86328125" customWidth="1"/>
+    <col min="8" max="8" width="15.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -4208,7 +4224,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>266</v>
       </c>
@@ -4234,7 +4250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>270</v>
       </c>
@@ -4260,7 +4276,7 @@
         <v>11.66</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>274</v>
       </c>
@@ -4286,7 +4302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>275</v>
       </c>
@@ -4312,7 +4328,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>279</v>
       </c>
@@ -4338,7 +4354,7 @@
         <v>9.65</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>283</v>
       </c>
@@ -4364,7 +4380,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
@@ -4390,7 +4406,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -4416,7 +4432,7 @@
         <v>9.6300000000000008</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>288</v>
       </c>
@@ -4442,7 +4458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>289</v>
       </c>
@@ -4468,7 +4484,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>291</v>
       </c>
@@ -4494,7 +4510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>295</v>
       </c>
@@ -4520,7 +4536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>299</v>
       </c>
@@ -4546,7 +4562,7 @@
         <v>10.57</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>

</xml_diff>